<commit_message>
Added logs to postgres database
</commit_message>
<xml_diff>
--- a/Review_Log.xlsx
+++ b/Review_Log.xlsx
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -583,14 +583,35 @@
         </is>
       </c>
       <c r="C6" s="5" t="n">
-        <v>45063.55024641076</v>
+        <v>45063.55024641204</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>45063.55029983558</v>
+        <v>45063.55029983796</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>C:/Users/gltig/OneDrive/Documents/GitHub/ReviewApp/Test</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>45063.85536992636</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>45063.85543055303</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>C:/Users/Alex/Documents/Builds/ReviewApp/Test</t>
         </is>
       </c>
     </row>

</xml_diff>